<commit_message>
Weapon and uren log
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="98">
   <si>
     <t>Maandag</t>
   </si>
@@ -302,6 +302,15 @@
   </si>
   <si>
     <t>Paco ziek</t>
+  </si>
+  <si>
+    <t>Roos en Danial kwartier te laat</t>
+  </si>
+  <si>
+    <t>goed doorgewerkt</t>
+  </si>
+  <si>
+    <t>kwartier te laat</t>
   </si>
 </sst>
 </file>
@@ -1341,7 +1350,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1351,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1360,20 +1369,20 @@
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="10.88671875" style="114" customWidth="1"/>
-    <col min="4" max="4" width="30.5546875" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="76.6640625" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="32.109375" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="70.88671875" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="40" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="58.6640625" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="40" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="42.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="30.5546875" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="10.88671875" style="114" customWidth="1"/>
+    <col min="6" max="6" width="76.6640625" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="10.88671875" style="114" customWidth="1"/>
+    <col min="8" max="8" width="32.109375" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="10.88671875" style="114" customWidth="1"/>
+    <col min="10" max="10" width="70.88671875" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="10.88671875" style="114" customWidth="1"/>
+    <col min="12" max="12" width="40" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="10.88671875" style="114" customWidth="1"/>
+    <col min="14" max="14" width="58.6640625" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="10.88671875" style="114" customWidth="1"/>
+    <col min="16" max="16" width="40" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="27.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="22.109375" style="7" customWidth="1"/>
     <col min="20" max="20" width="25.33203125" style="14" bestFit="1" customWidth="1"/>
@@ -1447,15 +1456,15 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="46">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="S2" s="62">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="T2" s="68">
         <f>S2/R2</f>
-        <v>0.96341463414634143</v>
+        <v>1.0116279069767442</v>
       </c>
       <c r="U2" s="57" t="str">
         <f>C1</f>
@@ -1515,11 +1524,11 @@
       <c r="R3" s="10"/>
       <c r="S3" s="63">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="T3" s="69">
         <f>S3/R2</f>
-        <v>0.8902439024390244</v>
+        <v>0.94186046511627908</v>
       </c>
       <c r="U3" s="58" t="str">
         <f>E1</f>
@@ -1579,11 +1588,11 @@
       <c r="R4" s="10"/>
       <c r="S4" s="64">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="T4" s="70">
         <f>S4/R2</f>
-        <v>0.92682926829268297</v>
+        <v>0.97674418604651159</v>
       </c>
       <c r="U4" s="59" t="str">
         <f>G1</f>
@@ -1643,11 +1652,11 @@
       <c r="R5" s="10"/>
       <c r="S5" s="65">
         <f>I8+I16+I24+I32+I47+I55+I63+I71+I79+I87+I95+I103+I118+I126+I134+I142+I150+I158+I166+I174</f>
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="T5" s="71">
         <f>S5/R2</f>
-        <v>1</v>
+        <v>1.0465116279069768</v>
       </c>
       <c r="U5" s="60" t="str">
         <f>I1</f>
@@ -1707,11 +1716,11 @@
       <c r="R6" s="10"/>
       <c r="S6" s="66">
         <f>K8+K16+K24+K32+K47+K55+K63+K71+K79+K87+K95+K103+K118+K126+K134+K142+K150+K158+K166+K174</f>
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="T6" s="72">
         <f>S6/R2</f>
-        <v>1</v>
+        <v>1.0465116279069768</v>
       </c>
       <c r="U6" s="40" t="str">
         <f>K1</f>
@@ -1763,11 +1772,11 @@
       <c r="R7" s="10"/>
       <c r="S7" s="67">
         <f>M8+M87+M24+M32+M47+M55+M63+M71+M79+M95+M103+M118+M126+M134+M142+M150+M158+M166+M174+M16</f>
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="T7" s="73">
         <f>S7/R2</f>
-        <v>0.91463414634146345</v>
+        <v>0.96511627906976749</v>
       </c>
       <c r="U7" s="61" t="str">
         <f>M1</f>
@@ -1821,11 +1830,11 @@
       <c r="R8" s="10"/>
       <c r="S8" s="52">
         <f>O8+O16+O24+O32+O47+O55+O63+O71+O79+O87+O95+O103+O118+O126+O134+O142+O150+O158+O166+O174</f>
-        <v>66.5</v>
+        <v>70.5</v>
       </c>
       <c r="T8" s="53">
         <f>S8/R2</f>
-        <v>0.81097560975609762</v>
+        <v>0.81976744186046513</v>
       </c>
       <c r="U8" s="56" t="str">
         <f>O1</f>
@@ -1875,7 +1884,7 @@
       </c>
       <c r="T10" s="41">
         <f>SUM(T2:T9)</f>
-        <v>6.5060975609756095</v>
+        <v>6.808139534883721</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3108,23 +3117,33 @@
       <c r="C44" s="48">
         <v>2</v>
       </c>
-      <c r="D44" s="49"/>
+      <c r="D44" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="E44" s="49">
         <v>2</v>
       </c>
-      <c r="F44" s="49"/>
+      <c r="F44" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="G44" s="49">
         <v>2</v>
       </c>
-      <c r="H44" s="49"/>
+      <c r="H44" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="I44" s="49">
         <v>2</v>
       </c>
-      <c r="J44" s="49"/>
+      <c r="J44" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="K44" s="49">
         <v>2</v>
       </c>
-      <c r="L44" s="49"/>
+      <c r="L44" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="M44" s="49">
         <v>0</v>
       </c>
@@ -3150,27 +3169,39 @@
       <c r="C45" s="48">
         <v>2</v>
       </c>
-      <c r="D45" s="49"/>
+      <c r="D45" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="E45" s="49">
         <v>2</v>
       </c>
-      <c r="F45" s="49"/>
+      <c r="F45" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="G45" s="49">
         <v>2</v>
       </c>
-      <c r="H45" s="49"/>
+      <c r="H45" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="I45" s="49">
         <v>2</v>
       </c>
-      <c r="J45" s="49"/>
+      <c r="J45" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="K45" s="49">
         <v>2</v>
       </c>
-      <c r="L45" s="49"/>
+      <c r="L45" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="M45" s="49">
         <v>2</v>
       </c>
-      <c r="N45" s="49"/>
+      <c r="N45" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="O45" s="50">
         <v>2</v>
       </c>
@@ -3182,36 +3213,54 @@
       <c r="A46" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="9"/>
+      <c r="B46" s="9">
+        <v>4</v>
+      </c>
       <c r="C46" s="108">
-        <v>0</v>
-      </c>
-      <c r="D46" s="106"/>
+        <v>4</v>
+      </c>
+      <c r="D46" s="106" t="s">
+        <v>96</v>
+      </c>
       <c r="E46" s="106">
-        <v>0</v>
-      </c>
-      <c r="F46" s="106"/>
+        <v>4</v>
+      </c>
+      <c r="F46" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="G46" s="106">
-        <v>0</v>
-      </c>
-      <c r="H46" s="106"/>
+        <v>4</v>
+      </c>
+      <c r="H46" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="I46" s="106">
-        <v>0</v>
-      </c>
-      <c r="J46" s="106"/>
+        <v>4</v>
+      </c>
+      <c r="J46" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="K46" s="106">
-        <v>0</v>
-      </c>
-      <c r="L46" s="106"/>
+        <v>4</v>
+      </c>
+      <c r="L46" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="M46" s="106">
-        <v>0</v>
-      </c>
-      <c r="N46" s="106"/>
+        <v>4</v>
+      </c>
+      <c r="N46" s="49" t="s">
+        <v>96</v>
+      </c>
       <c r="O46" s="107">
         <v>0</v>
       </c>
-      <c r="P46" s="107"/>
-      <c r="Q46" s="3"/>
+      <c r="P46" s="107" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q46" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="R46" s="10"/>
     </row>
     <row r="47" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3220,36 +3269,36 @@
       </c>
       <c r="B47" s="42">
         <f>SUM(B42:B46)</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C47" s="90">
         <f t="shared" ref="C47:K47" si="4">SUM(C42:C46)</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D47" s="91"/>
       <c r="E47" s="91">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F47" s="91"/>
       <c r="G47" s="91">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H47" s="91"/>
       <c r="I47" s="91">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J47" s="91"/>
       <c r="K47" s="91">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L47" s="91"/>
       <c r="M47" s="91">
         <f>SUM(M42:M46)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="N47" s="91"/>
       <c r="O47" s="91">
@@ -3260,7 +3309,7 @@
       <c r="Q47" s="39"/>
       <c r="R47" s="10"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C48" s="93"/>
       <c r="D48" s="93"/>
       <c r="E48" s="93"/>
@@ -3276,7 +3325,7 @@
       <c r="O48" s="93"/>
       <c r="P48" s="93"/>
     </row>
-    <row r="49" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>17</v>
       </c>
@@ -3298,43 +3347,51 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="10"/>
     </row>
-    <row r="50" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B50" s="10"/>
+      <c r="B50" s="10">
+        <v>4</v>
+      </c>
       <c r="C50" s="48">
-        <v>0</v>
-      </c>
-      <c r="D50" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="D50" s="49" t="s">
+        <v>97</v>
+      </c>
       <c r="E50" s="49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F50" s="49"/>
       <c r="G50" s="49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H50" s="49"/>
       <c r="I50" s="49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J50" s="49"/>
       <c r="K50" s="49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L50" s="49"/>
       <c r="M50" s="49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N50" s="49"/>
       <c r="O50" s="50">
-        <v>0</v>
-      </c>
-      <c r="P50" s="50"/>
-      <c r="Q50" s="2"/>
+        <v>4</v>
+      </c>
+      <c r="P50" s="50" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q50" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="R50" s="10"/>
     </row>
-    <row r="51" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>1</v>
       </c>
@@ -3370,7 +3427,7 @@
       <c r="Q51" s="2"/>
       <c r="R51" s="10"/>
     </row>
-    <row r="52" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>2</v>
       </c>
@@ -3406,7 +3463,7 @@
       <c r="Q52" s="2"/>
       <c r="R52" s="10"/>
     </row>
-    <row r="53" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>3</v>
       </c>
@@ -3442,7 +3499,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="10"/>
     </row>
-    <row r="54" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>4</v>
       </c>
@@ -3478,7 +3535,7 @@
       <c r="Q54" s="3"/>
       <c r="R54" s="10"/>
     </row>
-    <row r="55" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
         <v>5</v>
       </c>
@@ -3487,43 +3544,43 @@
       </c>
       <c r="C55" s="90">
         <f t="shared" ref="C55:K55" si="5">SUM(C50:C54)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D55" s="91"/>
       <c r="E55" s="91">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F55" s="91"/>
       <c r="G55" s="91">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H55" s="91"/>
       <c r="I55" s="91">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J55" s="91"/>
       <c r="K55" s="91">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L55" s="91"/>
       <c r="M55" s="91">
         <f>SUM(M50:M54)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N55" s="91"/>
       <c r="O55" s="92">
         <f>SUM(O50:O54)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P55" s="92"/>
       <c r="Q55" s="44"/>
       <c r="R55" s="10"/>
     </row>
-    <row r="56" spans="1:18" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C56" s="93"/>
       <c r="D56" s="93"/>
       <c r="E56" s="93"/>

</xml_diff>

<commit_message>
Uren Reg & weaponscript
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$D$1:$D$175</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$U$8</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="110">
   <si>
     <t>Maandag</t>
   </si>
@@ -1386,7 +1386,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1396,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1405,20 +1405,20 @@
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="10.88671875" style="114" customWidth="1"/>
-    <col min="4" max="4" width="30.5546875" style="114" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="10.88671875" style="114" customWidth="1"/>
-    <col min="6" max="6" width="76.6640625" style="114" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="10.88671875" style="114" customWidth="1"/>
-    <col min="8" max="8" width="32.109375" style="114" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="10.88671875" style="114" customWidth="1"/>
-    <col min="10" max="10" width="70.88671875" style="114" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="10.88671875" style="114" customWidth="1"/>
-    <col min="12" max="12" width="40" style="114" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="10.88671875" style="114" customWidth="1"/>
-    <col min="14" max="14" width="58.6640625" style="114" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="10.88671875" style="114" customWidth="1"/>
-    <col min="16" max="16" width="40" style="114" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="76.6640625" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.109375" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="70.88671875" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="40" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="58.6640625" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="40" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="42.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="27.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="22.109375" style="7" customWidth="1"/>
     <col min="20" max="20" width="25.33203125" style="14" bestFit="1" customWidth="1"/>
@@ -1470,7 +1470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1492,22 +1492,22 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="46">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="S2" s="62">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="T2" s="68">
         <f>S2/R2</f>
-        <v>0.96875</v>
+        <v>0.97</v>
       </c>
       <c r="U2" s="57" t="str">
         <f>C1</f>
         <v>Roos</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1564,14 +1564,14 @@
       </c>
       <c r="T3" s="69">
         <f>S3/R2</f>
-        <v>0.90625</v>
+        <v>0.87</v>
       </c>
       <c r="U3" s="58" t="str">
         <f>E1</f>
         <v>Harold</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1624,18 +1624,18 @@
       <c r="R4" s="10"/>
       <c r="S4" s="64">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="T4" s="70">
         <f>S4/R2</f>
-        <v>0.9375</v>
+        <v>0.94</v>
       </c>
       <c r="U4" s="59" t="str">
         <f>G1</f>
         <v>Patrick</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1688,18 +1688,18 @@
       <c r="R5" s="10"/>
       <c r="S5" s="65">
         <f>I8+I16+I24+I32+I47+I55+I63+I71+I79+I87+I95+I103+I118+I126+I134+I142+I150+I158+I166+I174</f>
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="T5" s="71">
         <f>S5/R2</f>
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="U5" s="60" t="str">
         <f>I1</f>
         <v>Erwin</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1752,7 +1752,7 @@
       <c r="R6" s="10"/>
       <c r="S6" s="66">
         <f>K8+K16+K24+K32+K47+K55+K63+K71+K79+K87+K95+K103+K118+K126+K134+K142+K150+K158+K166+K174</f>
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="T6" s="72">
         <f>S6/R2</f>
@@ -1763,7 +1763,7 @@
         <v>Sven</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1808,18 +1808,18 @@
       <c r="R7" s="10"/>
       <c r="S7" s="67">
         <f>M8+M87+M24+M32+M47+M55+M63+M71+M79+M95+M103+M118+M126+M134+M142+M150+M158+M166+M174+M16</f>
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="T7" s="73">
         <f>S7/R2</f>
-        <v>0.92708333333333337</v>
+        <v>0.93</v>
       </c>
       <c r="U7" s="61" t="str">
         <f>M1</f>
         <v>Paco</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -1866,18 +1866,18 @@
       <c r="R8" s="10"/>
       <c r="S8" s="52">
         <f>O8+O16+O24+O32+O47+O55+O63+O71+O79+O87+O95+O103+O118+O126+O134+O142+O150+O158+O166+O174</f>
-        <v>76.5</v>
+        <v>80.5</v>
       </c>
       <c r="T8" s="53">
         <f>S8/R2</f>
-        <v>0.796875</v>
+        <v>0.80500000000000005</v>
       </c>
       <c r="U8" s="56" t="str">
         <f>O1</f>
         <v>Danial</v>
       </c>
     </row>
-    <row r="9" spans="1:21" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C9" s="93"/>
       <c r="D9" s="93"/>
       <c r="E9" s="93"/>
@@ -1894,7 +1894,7 @@
       <c r="P9" s="93"/>
       <c r="Q9" s="15"/>
     </row>
-    <row r="10" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="79" t="s">
         <v>12</v>
       </c>
@@ -1920,10 +1920,10 @@
       </c>
       <c r="T10" s="41">
         <f>SUM(T2:T9)</f>
-        <v>6.536458333333333</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>6.4949999999999992</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="80" t="s">
         <v>0</v>
       </c>
@@ -1973,7 +1973,7 @@
       <c r="Q11" s="83"/>
       <c r="R11" s="10"/>
     </row>
-    <row r="12" spans="1:21" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A12" s="80" t="s">
         <v>1</v>
       </c>
@@ -2026,7 +2026,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:21" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A13" s="80" t="s">
         <v>2</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:21" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A14" s="80" t="s">
         <v>3</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="81" t="s">
         <v>4</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="81" t="s">
         <v>5</v>
       </c>
@@ -2236,7 +2236,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:18" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="93"/>
       <c r="D17" s="93"/>
       <c r="E17" s="93"/>
@@ -2253,7 +2253,7 @@
       <c r="P17" s="93"/>
       <c r="Q17" s="15"/>
     </row>
-    <row r="18" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -2275,7 +2275,7 @@
       <c r="Q18" s="82"/>
       <c r="R18" s="10"/>
     </row>
-    <row r="19" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
@@ -2325,7 +2325,7 @@
       <c r="Q19" s="83"/>
       <c r="R19" s="10"/>
     </row>
-    <row r="20" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>1</v>
       </c>
@@ -2368,7 +2368,7 @@
       <c r="N20" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="O20" s="49">
+      <c r="O20" s="50">
         <v>0</v>
       </c>
       <c r="P20" s="50"/>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="R20" s="10"/>
     </row>
-    <row r="21" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
@@ -2420,7 +2420,7 @@
       <c r="N21" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="O21" s="49">
+      <c r="O21" s="50">
         <v>0</v>
       </c>
       <c r="P21" s="50"/>
@@ -2429,7 +2429,7 @@
       </c>
       <c r="R21" s="10"/>
     </row>
-    <row r="22" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
@@ -2472,7 +2472,7 @@
       <c r="N22" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="O22" s="49">
+      <c r="O22" s="50">
         <v>0</v>
       </c>
       <c r="P22" s="50"/>
@@ -2481,7 +2481,7 @@
       </c>
       <c r="R22" s="10"/>
     </row>
-    <row r="23" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="R23" s="10"/>
     </row>
-    <row r="24" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>5</v>
       </c>
@@ -2575,7 +2575,7 @@
       <c r="Q24" s="39"/>
       <c r="R24" s="10"/>
     </row>
-    <row r="25" spans="1:18" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
       <c r="E25" s="93"/>
@@ -2591,7 +2591,7 @@
       <c r="O25" s="93"/>
       <c r="P25" s="93"/>
     </row>
-    <row r="26" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
@@ -2613,7 +2613,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="10"/>
     </row>
-    <row r="27" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
@@ -2653,7 +2653,7 @@
       </c>
       <c r="R27" s="10"/>
     </row>
-    <row r="28" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>1</v>
       </c>
@@ -2691,7 +2691,7 @@
       <c r="Q28" s="5"/>
       <c r="R28" s="10"/>
     </row>
-    <row r="29" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>2</v>
       </c>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="R29" s="10"/>
     </row>
-    <row r="30" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
@@ -2769,7 +2769,7 @@
       <c r="Q30" s="5"/>
       <c r="R30" s="10"/>
     </row>
-    <row r="31" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>4</v>
       </c>
@@ -2807,7 +2807,7 @@
       <c r="Q31" s="5"/>
       <c r="R31" s="10"/>
     </row>
-    <row r="32" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>5</v>
       </c>
@@ -2853,7 +2853,7 @@
       <c r="Q32" s="39"/>
       <c r="R32" s="10"/>
     </row>
-    <row r="33" spans="1:18" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33" s="93"/>
       <c r="D33" s="93"/>
       <c r="E33" s="93"/>
@@ -3531,11 +3531,15 @@
       <c r="A53" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B53" s="10"/>
+      <c r="B53" s="10">
+        <v>2</v>
+      </c>
       <c r="C53" s="48">
-        <v>0</v>
-      </c>
-      <c r="D53" s="49"/>
+        <v>2</v>
+      </c>
+      <c r="D53" s="49" t="s">
+        <v>100</v>
+      </c>
       <c r="E53" s="49">
         <v>0</v>
       </c>
@@ -3543,25 +3547,31 @@
         <v>108</v>
       </c>
       <c r="G53" s="49">
-        <v>0</v>
-      </c>
-      <c r="H53" s="49"/>
+        <v>2</v>
+      </c>
+      <c r="H53" s="49" t="s">
+        <v>100</v>
+      </c>
       <c r="I53" s="49">
         <v>0</v>
       </c>
-      <c r="J53" s="49"/>
+      <c r="J53" s="49" t="s">
+        <v>109</v>
+      </c>
       <c r="K53" s="49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L53" s="49" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="M53" s="49">
-        <v>0</v>
-      </c>
-      <c r="N53" s="49"/>
+        <v>2</v>
+      </c>
+      <c r="N53" s="49" t="s">
+        <v>100</v>
+      </c>
       <c r="O53" s="50">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P53" s="50"/>
       <c r="Q53" s="2"/>
@@ -3571,11 +3581,15 @@
       <c r="A54" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B54" s="9"/>
+      <c r="B54" s="9">
+        <v>2</v>
+      </c>
       <c r="C54" s="108">
-        <v>0</v>
-      </c>
-      <c r="D54" s="106"/>
+        <v>2</v>
+      </c>
+      <c r="D54" s="49" t="s">
+        <v>100</v>
+      </c>
       <c r="E54" s="106">
         <v>0</v>
       </c>
@@ -3583,23 +3597,31 @@
         <v>108</v>
       </c>
       <c r="G54" s="106">
-        <v>0</v>
-      </c>
-      <c r="H54" s="106"/>
+        <v>2</v>
+      </c>
+      <c r="H54" s="49" t="s">
+        <v>100</v>
+      </c>
       <c r="I54" s="106">
-        <v>0</v>
-      </c>
-      <c r="J54" s="106"/>
+        <v>2</v>
+      </c>
+      <c r="J54" s="49" t="s">
+        <v>100</v>
+      </c>
       <c r="K54" s="106">
-        <v>0</v>
-      </c>
-      <c r="L54" s="106"/>
+        <v>2</v>
+      </c>
+      <c r="L54" s="49" t="s">
+        <v>100</v>
+      </c>
       <c r="M54" s="106">
-        <v>0</v>
-      </c>
-      <c r="N54" s="106"/>
+        <v>2</v>
+      </c>
+      <c r="N54" s="49" t="s">
+        <v>100</v>
+      </c>
       <c r="O54" s="107">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P54" s="107"/>
       <c r="Q54" s="3"/>
@@ -3611,11 +3633,11 @@
       </c>
       <c r="B55" s="46">
         <f>SUM(B50:B54)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C55" s="90">
         <f t="shared" ref="C55:K55" si="5">SUM(C50:C54)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D55" s="91"/>
       <c r="E55" s="91">
@@ -3625,27 +3647,27 @@
       <c r="F55" s="91"/>
       <c r="G55" s="91">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H55" s="91"/>
       <c r="I55" s="91">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J55" s="91"/>
       <c r="K55" s="91">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="L55" s="91"/>
       <c r="M55" s="91">
         <f>SUM(M50:M54)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="N55" s="91"/>
       <c r="O55" s="92">
         <f>SUM(O50:O54)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P55" s="92"/>
       <c r="Q55" s="44"/>

</xml_diff>

<commit_message>
urenlog & gdd & weapon & enemy creator
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="111">
   <si>
     <t>Maandag</t>
   </si>
@@ -334,12 +334,6 @@
     <t>Goed bezig</t>
   </si>
   <si>
-    <t>Thuis bezig</t>
-  </si>
-  <si>
-    <t>Git hub problemen</t>
-  </si>
-  <si>
     <t>Thuis bezig, mummy rig af mummy normal map torch particle</t>
   </si>
   <si>
@@ -347,6 +341,15 @@
   </si>
   <si>
     <t>rijexamen</t>
+  </si>
+  <si>
+    <t>Git hub problemen, wel gewerkt</t>
+  </si>
+  <si>
+    <t>Thuis bezig, weapon uv</t>
+  </si>
+  <si>
+    <t>Goed gewerkt, heeft zich aankunnen passen aan scripts waarvan hij een ander idee van aanpak had</t>
   </si>
 </sst>
 </file>
@@ -1386,7 +1389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1396,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1405,18 +1408,18 @@
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="10.88671875" style="114" customWidth="1"/>
-    <col min="4" max="4" width="30.5546875" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="76.6640625" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="32.109375" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="70.88671875" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="40" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="58.6640625" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.88671875" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="10.88671875" style="114" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="10.88671875" style="114" customWidth="1"/>
+    <col min="8" max="8" width="29.44140625" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="10.88671875" style="114" customWidth="1"/>
+    <col min="10" max="10" width="30.21875" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="10.88671875" style="114" customWidth="1"/>
+    <col min="12" max="12" width="28.33203125" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="10.88671875" style="114" customWidth="1"/>
+    <col min="14" max="14" width="35.44140625" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="10.88671875" style="114" customWidth="1"/>
     <col min="16" max="16" width="40" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="17" max="17" width="42.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="27.6640625" style="7" bestFit="1" customWidth="1"/>
@@ -1492,15 +1495,15 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="46">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="S2" s="62">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="T2" s="68">
         <f>S2/R2</f>
-        <v>0.97</v>
+        <v>0.97115384615384615</v>
       </c>
       <c r="U2" s="57" t="str">
         <f>C1</f>
@@ -1560,11 +1563,11 @@
       <c r="R3" s="10"/>
       <c r="S3" s="63">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="T3" s="69">
         <f>S3/R2</f>
-        <v>0.87</v>
+        <v>0.875</v>
       </c>
       <c r="U3" s="58" t="str">
         <f>E1</f>
@@ -1624,11 +1627,11 @@
       <c r="R4" s="10"/>
       <c r="S4" s="64">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="T4" s="70">
         <f>S4/R2</f>
-        <v>0.94</v>
+        <v>0.94230769230769229</v>
       </c>
       <c r="U4" s="59" t="str">
         <f>G1</f>
@@ -1688,11 +1691,11 @@
       <c r="R5" s="10"/>
       <c r="S5" s="65">
         <f>I8+I16+I24+I32+I47+I55+I63+I71+I79+I87+I95+I103+I118+I126+I134+I142+I150+I158+I166+I174</f>
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="T5" s="71">
         <f>S5/R2</f>
-        <v>0.98</v>
+        <v>0.98076923076923073</v>
       </c>
       <c r="U5" s="60" t="str">
         <f>I1</f>
@@ -1752,7 +1755,7 @@
       <c r="R6" s="10"/>
       <c r="S6" s="66">
         <f>K8+K16+K24+K32+K47+K55+K63+K71+K79+K87+K95+K103+K118+K126+K134+K142+K150+K158+K166+K174</f>
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="T6" s="72">
         <f>S6/R2</f>
@@ -1808,11 +1811,11 @@
       <c r="R7" s="10"/>
       <c r="S7" s="67">
         <f>M8+M87+M24+M32+M47+M55+M63+M71+M79+M95+M103+M118+M126+M134+M142+M150+M158+M166+M174+M16</f>
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="T7" s="73">
         <f>S7/R2</f>
-        <v>0.93</v>
+        <v>0.93269230769230771</v>
       </c>
       <c r="U7" s="61" t="str">
         <f>M1</f>
@@ -1870,14 +1873,14 @@
       </c>
       <c r="T8" s="53">
         <f>S8/R2</f>
-        <v>0.80500000000000005</v>
+        <v>0.77403846153846156</v>
       </c>
       <c r="U8" s="56" t="str">
         <f>O1</f>
         <v>Danial</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C9" s="93"/>
       <c r="D9" s="93"/>
       <c r="E9" s="93"/>
@@ -1894,7 +1897,7 @@
       <c r="P9" s="93"/>
       <c r="Q9" s="15"/>
     </row>
-    <row r="10" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="79" t="s">
         <v>12</v>
       </c>
@@ -1920,10 +1923,10 @@
       </c>
       <c r="T10" s="41">
         <f>SUM(T2:T9)</f>
-        <v>6.4949999999999992</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>6.4759615384615383</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="80" t="s">
         <v>0</v>
       </c>
@@ -1973,7 +1976,7 @@
       <c r="Q11" s="83"/>
       <c r="R11" s="10"/>
     </row>
-    <row r="12" spans="1:21" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A12" s="80" t="s">
         <v>1</v>
       </c>
@@ -2026,7 +2029,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:21" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A13" s="80" t="s">
         <v>2</v>
       </c>
@@ -2079,7 +2082,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:21" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A14" s="80" t="s">
         <v>3</v>
       </c>
@@ -2132,7 +2135,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="81" t="s">
         <v>4</v>
       </c>
@@ -2187,7 +2190,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="81" t="s">
         <v>5</v>
       </c>
@@ -2236,7 +2239,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" collapsed="1" x14ac:dyDescent="0.3">
       <c r="C17" s="93"/>
       <c r="D17" s="93"/>
       <c r="E17" s="93"/>
@@ -2253,7 +2256,7 @@
       <c r="P17" s="93"/>
       <c r="Q17" s="15"/>
     </row>
-    <row r="18" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -2275,7 +2278,7 @@
       <c r="Q18" s="82"/>
       <c r="R18" s="10"/>
     </row>
-    <row r="19" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
@@ -2325,7 +2328,7 @@
       <c r="Q19" s="83"/>
       <c r="R19" s="10"/>
     </row>
-    <row r="20" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>1</v>
       </c>
@@ -2377,7 +2380,7 @@
       </c>
       <c r="R20" s="10"/>
     </row>
-    <row r="21" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>2</v>
       </c>
@@ -2429,7 +2432,7 @@
       </c>
       <c r="R21" s="10"/>
     </row>
-    <row r="22" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>3</v>
       </c>
@@ -2481,7 +2484,7 @@
       </c>
       <c r="R22" s="10"/>
     </row>
-    <row r="23" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
@@ -2529,7 +2532,7 @@
       </c>
       <c r="R23" s="10"/>
     </row>
-    <row r="24" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>5</v>
       </c>
@@ -2575,7 +2578,7 @@
       <c r="Q24" s="39"/>
       <c r="R24" s="10"/>
     </row>
-    <row r="25" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" collapsed="1" x14ac:dyDescent="0.3">
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
       <c r="E25" s="93"/>
@@ -2591,7 +2594,7 @@
       <c r="O25" s="93"/>
       <c r="P25" s="93"/>
     </row>
-    <row r="26" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
@@ -2613,7 +2616,7 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="10"/>
     </row>
-    <row r="27" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>0</v>
       </c>
@@ -2653,7 +2656,7 @@
       </c>
       <c r="R27" s="10"/>
     </row>
-    <row r="28" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>1</v>
       </c>
@@ -2691,7 +2694,7 @@
       <c r="Q28" s="5"/>
       <c r="R28" s="10"/>
     </row>
-    <row r="29" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>2</v>
       </c>
@@ -2731,7 +2734,7 @@
       </c>
       <c r="R29" s="10"/>
     </row>
-    <row r="30" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
@@ -2769,7 +2772,7 @@
       <c r="Q30" s="5"/>
       <c r="R30" s="10"/>
     </row>
-    <row r="31" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>4</v>
       </c>
@@ -2807,7 +2810,7 @@
       <c r="Q31" s="5"/>
       <c r="R31" s="10"/>
     </row>
-    <row r="32" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>5</v>
       </c>
@@ -2853,7 +2856,7 @@
       <c r="Q32" s="39"/>
       <c r="R32" s="10"/>
     </row>
-    <row r="33" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33" s="93"/>
       <c r="D33" s="93"/>
       <c r="E33" s="93"/>
@@ -3506,19 +3509,19 @@
         <v>2</v>
       </c>
       <c r="J52" s="49" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K52" s="49">
         <v>2</v>
       </c>
       <c r="L52" s="49" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="M52" s="49">
         <v>2</v>
       </c>
       <c r="N52" s="49" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="O52" s="50">
         <v>2</v>
@@ -3544,7 +3547,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="49" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G53" s="49">
         <v>2</v>
@@ -3556,7 +3559,7 @@
         <v>0</v>
       </c>
       <c r="J53" s="49" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K53" s="49">
         <v>2</v>
@@ -3594,7 +3597,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="49" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G54" s="106">
         <v>2</v>
@@ -3673,7 +3676,7 @@
       <c r="Q55" s="44"/>
       <c r="R55" s="10"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C56" s="93"/>
       <c r="D56" s="93"/>
       <c r="E56" s="93"/>
@@ -3689,7 +3692,7 @@
       <c r="O56" s="93"/>
       <c r="P56" s="93"/>
     </row>
-    <row r="57" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>18</v>
       </c>
@@ -3711,35 +3714,49 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="10"/>
     </row>
-    <row r="58" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="10"/>
+      <c r="B58" s="10">
+        <v>4</v>
+      </c>
       <c r="C58" s="48">
-        <v>0</v>
-      </c>
-      <c r="D58" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="D58" s="49" t="s">
+        <v>100</v>
+      </c>
       <c r="E58" s="49">
-        <v>0</v>
-      </c>
-      <c r="F58" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="F58" s="49" t="s">
+        <v>110</v>
+      </c>
       <c r="G58" s="49">
-        <v>0</v>
-      </c>
-      <c r="H58" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="H58" s="49" t="s">
+        <v>87</v>
+      </c>
       <c r="I58" s="49">
-        <v>0</v>
-      </c>
-      <c r="J58" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="J58" s="49" t="s">
+        <v>87</v>
+      </c>
       <c r="K58" s="49">
-        <v>0</v>
-      </c>
-      <c r="L58" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="L58" s="49" t="s">
+        <v>87</v>
+      </c>
       <c r="M58" s="49">
-        <v>0</v>
-      </c>
-      <c r="N58" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="N58" s="49" t="s">
+        <v>87</v>
+      </c>
       <c r="O58" s="50">
         <v>0</v>
       </c>
@@ -3747,7 +3764,7 @@
       <c r="Q58" s="2"/>
       <c r="R58" s="10"/>
     </row>
-    <row r="59" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>1</v>
       </c>
@@ -3783,7 +3800,7 @@
       <c r="Q59" s="2"/>
       <c r="R59" s="10"/>
     </row>
-    <row r="60" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>2</v>
       </c>
@@ -3819,7 +3836,7 @@
       <c r="Q60" s="2"/>
       <c r="R60" s="10"/>
     </row>
-    <row r="61" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>3</v>
       </c>
@@ -3855,7 +3872,7 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="10"/>
     </row>
-    <row r="62" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="6" t="s">
         <v>4</v>
       </c>
@@ -3891,41 +3908,42 @@
       <c r="Q62" s="3"/>
       <c r="R62" s="10"/>
     </row>
-    <row r="63" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B63" s="46">
-        <v>0</v>
+        <f>SUM(B58:B62)</f>
+        <v>4</v>
       </c>
       <c r="C63" s="90">
         <f t="shared" ref="C63:K63" si="6">SUM(C58:C62)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D63" s="91"/>
       <c r="E63" s="91">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F63" s="91"/>
       <c r="G63" s="91">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H63" s="91"/>
       <c r="I63" s="91">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J63" s="91"/>
       <c r="K63" s="91">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L63" s="91"/>
       <c r="M63" s="91">
         <f>SUM(M58:M62)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N63" s="91"/>
       <c r="O63" s="92">
@@ -3936,7 +3954,7 @@
       <c r="Q63" s="39"/>
       <c r="R63" s="10"/>
     </row>
-    <row r="64" spans="1:18" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B64" s="10"/>
       <c r="C64" s="109"/>
       <c r="D64" s="109"/>

</xml_diff>

<commit_message>
Weapon script & urenlog
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="112">
   <si>
     <t>Maandag</t>
   </si>
@@ -350,6 +350,9 @@
   </si>
   <si>
     <t>Goed gewerkt, heeft zich aankunnen passen aan scripts waarvan hij een ander idee van aanpak had</t>
+  </si>
+  <si>
+    <t>Geen opmerking, ik was er niet</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1392,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1399,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1495,15 +1498,15 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="46">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="S2" s="62">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="T2" s="68">
         <f>S2/R2</f>
-        <v>0.97115384615384615</v>
+        <v>0.97222222222222221</v>
       </c>
       <c r="U2" s="57" t="str">
         <f>C1</f>
@@ -1563,11 +1566,11 @@
       <c r="R3" s="10"/>
       <c r="S3" s="63">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="T3" s="69">
         <f>S3/R2</f>
-        <v>0.875</v>
+        <v>0.87962962962962965</v>
       </c>
       <c r="U3" s="58" t="str">
         <f>E1</f>
@@ -1627,11 +1630,11 @@
       <c r="R4" s="10"/>
       <c r="S4" s="64">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="T4" s="70">
         <f>S4/R2</f>
-        <v>0.94230769230769229</v>
+        <v>0.94444444444444442</v>
       </c>
       <c r="U4" s="59" t="str">
         <f>G1</f>
@@ -1691,11 +1694,11 @@
       <c r="R5" s="10"/>
       <c r="S5" s="65">
         <f>I8+I16+I24+I32+I47+I55+I63+I71+I79+I87+I95+I103+I118+I126+I134+I142+I150+I158+I166+I174</f>
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="T5" s="71">
         <f>S5/R2</f>
-        <v>0.98076923076923073</v>
+        <v>0.98148148148148151</v>
       </c>
       <c r="U5" s="60" t="str">
         <f>I1</f>
@@ -1755,7 +1758,7 @@
       <c r="R6" s="10"/>
       <c r="S6" s="66">
         <f>K8+K16+K24+K32+K47+K55+K63+K71+K79+K87+K95+K103+K118+K126+K134+K142+K150+K158+K166+K174</f>
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="T6" s="72">
         <f>S6/R2</f>
@@ -1811,11 +1814,11 @@
       <c r="R7" s="10"/>
       <c r="S7" s="67">
         <f>M8+M87+M24+M32+M47+M55+M63+M71+M79+M95+M103+M118+M126+M134+M142+M150+M158+M166+M174+M16</f>
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="T7" s="73">
         <f>S7/R2</f>
-        <v>0.93269230769230771</v>
+        <v>0.93518518518518523</v>
       </c>
       <c r="U7" s="61" t="str">
         <f>M1</f>
@@ -1873,7 +1876,7 @@
       </c>
       <c r="T8" s="53">
         <f>S8/R2</f>
-        <v>0.77403846153846156</v>
+        <v>0.74537037037037035</v>
       </c>
       <c r="U8" s="56" t="str">
         <f>O1</f>
@@ -1923,7 +1926,7 @@
       </c>
       <c r="T10" s="41">
         <f>SUM(T2:T9)</f>
-        <v>6.4759615384615383</v>
+        <v>6.458333333333333</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3768,31 +3771,45 @@
       <c r="A59" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B59" s="10"/>
+      <c r="B59" s="10">
+        <v>4</v>
+      </c>
       <c r="C59" s="48">
-        <v>0</v>
-      </c>
-      <c r="D59" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="D59" s="49" t="s">
+        <v>111</v>
+      </c>
       <c r="E59" s="49">
-        <v>0</v>
-      </c>
-      <c r="F59" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="F59" s="49" t="s">
+        <v>111</v>
+      </c>
       <c r="G59" s="49">
-        <v>0</v>
-      </c>
-      <c r="H59" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="H59" s="49" t="s">
+        <v>111</v>
+      </c>
       <c r="I59" s="49">
-        <v>0</v>
-      </c>
-      <c r="J59" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="J59" s="49" t="s">
+        <v>111</v>
+      </c>
       <c r="K59" s="49">
-        <v>0</v>
-      </c>
-      <c r="L59" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="L59" s="49" t="s">
+        <v>111</v>
+      </c>
       <c r="M59" s="49">
-        <v>0</v>
-      </c>
-      <c r="N59" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="N59" s="49" t="s">
+        <v>111</v>
+      </c>
       <c r="O59" s="50">
         <v>0</v>
       </c>
@@ -3914,36 +3931,36 @@
       </c>
       <c r="B63" s="46">
         <f>SUM(B58:B62)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C63" s="90">
         <f t="shared" ref="C63:K63" si="6">SUM(C58:C62)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D63" s="91"/>
       <c r="E63" s="91">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F63" s="91"/>
       <c r="G63" s="91">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H63" s="91"/>
       <c r="I63" s="91">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J63" s="91"/>
       <c r="K63" s="91">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L63" s="91"/>
       <c r="M63" s="91">
         <f>SUM(M58:M62)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N63" s="91"/>
       <c r="O63" s="92">

</xml_diff>

<commit_message>
weapon fix & urenlog
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="123">
   <si>
     <t>Maandag</t>
   </si>
@@ -371,6 +371,21 @@
   </si>
   <si>
     <t>Heb tot 17.15 op school gezeten voor gamelab</t>
+  </si>
+  <si>
+    <t>drie kwartier te laat</t>
+  </si>
+  <si>
+    <t>Harold ziek</t>
+  </si>
+  <si>
+    <t>Harold ziek, danial kwartier te laat, paco drie kwartier te laat</t>
+  </si>
+  <si>
+    <t>ziek</t>
+  </si>
+  <si>
+    <t>ziek, zou proberen thuis te werken</t>
   </si>
 </sst>
 </file>
@@ -784,7 +799,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -1132,6 +1147,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1410,7 +1428,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1420,8 +1438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q66" sqref="Q66"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q67" sqref="Q67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1441,8 +1459,8 @@
     <col min="13" max="13" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="35.44140625" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="15" max="15" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="40" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="42.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="40" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="27.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="22.109375" style="7" customWidth="1"/>
     <col min="20" max="20" width="25.33203125" style="14" bestFit="1" customWidth="1"/>
@@ -1516,15 +1534,15 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="46">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="S2" s="62">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="T2" s="68">
         <f>S2/R2</f>
-        <v>0.9732142857142857</v>
+        <v>0.97457627118644063</v>
       </c>
       <c r="U2" s="57" t="str">
         <f>C1</f>
@@ -1588,7 +1606,7 @@
       </c>
       <c r="T3" s="69">
         <f>S3/R2</f>
-        <v>0.8839285714285714</v>
+        <v>0.83898305084745761</v>
       </c>
       <c r="U3" s="58" t="str">
         <f>E1</f>
@@ -1648,11 +1666,11 @@
       <c r="R4" s="10"/>
       <c r="S4" s="64">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="T4" s="70">
         <f>S4/R2</f>
-        <v>0.9464285714285714</v>
+        <v>0.94915254237288138</v>
       </c>
       <c r="U4" s="59" t="str">
         <f>G1</f>
@@ -1712,11 +1730,11 @@
       <c r="R5" s="10"/>
       <c r="S5" s="65">
         <f>I8+I16+I24+I32+I47+I55+I63+I71+I79+I87+I95+I103+I118+I126+I134+I142+I150+I158+I166+I174</f>
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="T5" s="71">
         <f>S5/R2</f>
-        <v>0.9821428571428571</v>
+        <v>0.98305084745762716</v>
       </c>
       <c r="U5" s="60" t="str">
         <f>I1</f>
@@ -1776,7 +1794,7 @@
       <c r="R6" s="10"/>
       <c r="S6" s="66">
         <f>K8+K16+K24+K32+K47+K55+K63+K71+K79+K87+K95+K103+K118+K126+K134+K142+K150+K158+K166+K174</f>
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="T6" s="72">
         <f>S6/R2</f>
@@ -1832,11 +1850,11 @@
       <c r="R7" s="10"/>
       <c r="S7" s="67">
         <f>M8+M87+M24+M32+M47+M55+M63+M71+M79+M95+M103+M118+M126+M134+M142+M150+M158+M166+M174+M16</f>
-        <v>105</v>
+        <v>110.15</v>
       </c>
       <c r="T7" s="73">
         <f>S7/R2</f>
-        <v>0.9375</v>
+        <v>0.93347457627118646</v>
       </c>
       <c r="U7" s="61" t="str">
         <f>M1</f>
@@ -1890,11 +1908,11 @@
       <c r="R8" s="10"/>
       <c r="S8" s="52">
         <f>O8+O16+O24+O32+O47+O55+O63+O71+O79+O87+O95+O103+O118+O126+O134+O142+O150+O158+O166+O174</f>
-        <v>88</v>
+        <v>93.75</v>
       </c>
       <c r="T8" s="53">
         <f>S8/R2</f>
-        <v>0.7857142857142857</v>
+        <v>0.79449152542372881</v>
       </c>
       <c r="U8" s="56" t="str">
         <f>O1</f>
@@ -1944,7 +1962,7 @@
       </c>
       <c r="T10" s="41">
         <f>SUM(T2:T9)</f>
-        <v>6.5089285714285721</v>
+        <v>6.4737288135593225</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -3027,7 +3045,7 @@
       <c r="Q39" s="21"/>
       <c r="R39" s="10"/>
     </row>
-    <row r="40" spans="1:18" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" collapsed="1" x14ac:dyDescent="0.3">
       <c r="C40" s="93"/>
       <c r="D40" s="93"/>
       <c r="E40" s="93"/>
@@ -3043,7 +3061,7 @@
       <c r="O40" s="93"/>
       <c r="P40" s="93"/>
     </row>
-    <row r="41" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>16</v>
       </c>
@@ -3065,7 +3083,7 @@
       <c r="Q41" s="1"/>
       <c r="R41" s="10"/>
     </row>
-    <row r="42" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>0</v>
       </c>
@@ -3117,7 +3135,7 @@
       <c r="Q42" s="2"/>
       <c r="R42" s="10"/>
     </row>
-    <row r="43" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>1</v>
       </c>
@@ -3167,7 +3185,7 @@
       <c r="Q43" s="2"/>
       <c r="R43" s="10"/>
     </row>
-    <row r="44" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>2</v>
       </c>
@@ -3219,7 +3237,7 @@
       </c>
       <c r="R44" s="10"/>
     </row>
-    <row r="45" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>3</v>
       </c>
@@ -3269,7 +3287,7 @@
       <c r="Q45" s="2"/>
       <c r="R45" s="10"/>
     </row>
-    <row r="46" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
         <v>4</v>
       </c>
@@ -3323,7 +3341,7 @@
       </c>
       <c r="R46" s="10"/>
     </row>
-    <row r="47" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
         <v>5</v>
       </c>
@@ -3369,7 +3387,7 @@
       <c r="Q47" s="39"/>
       <c r="R47" s="10"/>
     </row>
-    <row r="48" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" collapsed="1" x14ac:dyDescent="0.3">
       <c r="C48" s="93"/>
       <c r="D48" s="93"/>
       <c r="E48" s="93"/>
@@ -3385,7 +3403,7 @@
       <c r="O48" s="93"/>
       <c r="P48" s="93"/>
     </row>
-    <row r="49" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>17</v>
       </c>
@@ -3407,7 +3425,7 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="10"/>
     </row>
-    <row r="50" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>0</v>
       </c>
@@ -3451,7 +3469,7 @@
       </c>
       <c r="R50" s="10"/>
     </row>
-    <row r="51" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>1</v>
       </c>
@@ -3501,7 +3519,7 @@
       <c r="Q51" s="2"/>
       <c r="R51" s="10"/>
     </row>
-    <row r="52" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>2</v>
       </c>
@@ -3551,7 +3569,7 @@
       <c r="Q52" s="2"/>
       <c r="R52" s="10"/>
     </row>
-    <row r="53" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
         <v>3</v>
       </c>
@@ -3601,7 +3619,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="10"/>
     </row>
-    <row r="54" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>4</v>
       </c>
@@ -3653,7 +3671,7 @@
       <c r="Q54" s="3"/>
       <c r="R54" s="10"/>
     </row>
-    <row r="55" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="6" t="s">
         <v>5</v>
       </c>
@@ -3699,7 +3717,7 @@
       <c r="Q55" s="44"/>
       <c r="R55" s="10"/>
     </row>
-    <row r="56" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:18" ht="15" collapsed="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C56" s="93"/>
       <c r="D56" s="93"/>
       <c r="E56" s="93"/>
@@ -4088,7 +4106,7 @@
       <c r="A66" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B66" s="36" t="s">
+      <c r="B66" s="137" t="s">
         <v>112</v>
       </c>
       <c r="C66" s="48">
@@ -4126,7 +4144,7 @@
       <c r="A67" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B67" s="36" t="s">
+      <c r="B67" s="137" t="s">
         <v>112</v>
       </c>
       <c r="C67" s="48">
@@ -4164,7 +4182,7 @@
       <c r="A68" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B68" s="36" t="s">
+      <c r="B68" s="137" t="s">
         <v>112</v>
       </c>
       <c r="C68" s="48">
@@ -4202,72 +4220,88 @@
       <c r="A69" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B69" s="36"/>
+      <c r="B69" s="36">
+        <v>2</v>
+      </c>
       <c r="C69" s="48">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D69" s="49"/>
       <c r="E69" s="49">
         <v>0</v>
       </c>
-      <c r="F69" s="49"/>
+      <c r="F69" s="49" t="s">
+        <v>121</v>
+      </c>
       <c r="G69" s="49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H69" s="49"/>
       <c r="I69" s="49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J69" s="49"/>
       <c r="K69" s="49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L69" s="49"/>
       <c r="M69" s="49">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N69" s="49"/>
       <c r="O69" s="50">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P69" s="50"/>
-      <c r="Q69" s="26"/>
+      <c r="Q69" s="26" t="s">
+        <v>119</v>
+      </c>
       <c r="R69" s="10"/>
     </row>
     <row r="70" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B70" s="37"/>
+      <c r="B70" s="37">
+        <v>4</v>
+      </c>
       <c r="C70" s="108">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D70" s="106"/>
       <c r="E70" s="106">
         <v>0</v>
       </c>
-      <c r="F70" s="106"/>
+      <c r="F70" s="106" t="s">
+        <v>122</v>
+      </c>
       <c r="G70" s="106">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H70" s="106"/>
       <c r="I70" s="106">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J70" s="106"/>
       <c r="K70" s="106">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L70" s="106"/>
       <c r="M70" s="106">
-        <v>0</v>
-      </c>
-      <c r="N70" s="106"/>
+        <v>3.15</v>
+      </c>
+      <c r="N70" s="106" t="s">
+        <v>118</v>
+      </c>
       <c r="O70" s="107">
-        <v>0</v>
-      </c>
-      <c r="P70" s="107"/>
-      <c r="Q70" s="28"/>
+        <v>3.75</v>
+      </c>
+      <c r="P70" s="107" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q70" s="28" t="s">
+        <v>120</v>
+      </c>
       <c r="R70" s="10"/>
     </row>
     <row r="71" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4275,11 +4309,12 @@
         <v>5</v>
       </c>
       <c r="B71" s="46">
-        <v>0</v>
+        <f>SUM(B69:B70)</f>
+        <v>6</v>
       </c>
       <c r="C71" s="90">
         <f t="shared" ref="C71:K71" si="7">SUM(C66:C70)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D71" s="91"/>
       <c r="E71" s="91">
@@ -4289,33 +4324,33 @@
       <c r="F71" s="91"/>
       <c r="G71" s="91">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H71" s="91"/>
       <c r="I71" s="91">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J71" s="91"/>
       <c r="K71" s="91">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L71" s="91"/>
       <c r="M71" s="91">
         <f>SUM(M66:M70)</f>
-        <v>0</v>
+        <v>5.15</v>
       </c>
       <c r="N71" s="91"/>
       <c r="O71" s="92">
         <f>SUM(O66:O70)</f>
-        <v>0</v>
+        <v>5.75</v>
       </c>
       <c r="P71" s="92"/>
       <c r="Q71" s="44"/>
       <c r="R71" s="10"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C72" s="93"/>
       <c r="D72" s="93"/>
       <c r="E72" s="93"/>
@@ -4331,7 +4366,7 @@
       <c r="O72" s="93"/>
       <c r="P72" s="93"/>
     </row>
-    <row r="73" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>20</v>
       </c>
@@ -4353,7 +4388,7 @@
       <c r="Q73" s="1"/>
       <c r="R73" s="10"/>
     </row>
-    <row r="74" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>0</v>
       </c>
@@ -4389,7 +4424,7 @@
       <c r="Q74" s="2"/>
       <c r="R74" s="10"/>
     </row>
-    <row r="75" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>1</v>
       </c>
@@ -4425,7 +4460,7 @@
       <c r="Q75" s="2"/>
       <c r="R75" s="10"/>
     </row>
-    <row r="76" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>2</v>
       </c>
@@ -4461,7 +4496,7 @@
       <c r="Q76" s="2"/>
       <c r="R76" s="10"/>
     </row>
-    <row r="77" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>3</v>
       </c>
@@ -4497,7 +4532,7 @@
       <c r="Q77" s="2"/>
       <c r="R77" s="10"/>
     </row>
-    <row r="78" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="6" t="s">
         <v>4</v>
       </c>
@@ -4533,7 +4568,7 @@
       <c r="Q78" s="3"/>
       <c r="R78" s="10"/>
     </row>
-    <row r="79" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="6" t="s">
         <v>5</v>
       </c>
@@ -4578,7 +4613,7 @@
       <c r="Q79" s="44"/>
       <c r="R79" s="10"/>
     </row>
-    <row r="80" spans="1:18" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C80" s="93"/>
       <c r="D80" s="93"/>
       <c r="E80" s="93"/>

</xml_diff>

<commit_message>
Uren log & weaponscript
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="133">
   <si>
     <t>Maandag</t>
   </si>
@@ -386,6 +386,36 @@
   </si>
   <si>
     <t>ziek, zou proberen thuis te werken</t>
+  </si>
+  <si>
+    <t>kwartier te laat, tot 17.15 op school gezet voor gamelab</t>
+  </si>
+  <si>
+    <t>goed gewerkt, nam de feedback op haar workflow goed op</t>
+  </si>
+  <si>
+    <t>goed gewerkt laat vaak van zijn werk dingen zien</t>
+  </si>
+  <si>
+    <t>goed gewerkt, toonde initiatatief voor meer werk heb met hem een kleine persoonlijke planning gemaakt voor extra assets waarin ik hem begelijd</t>
+  </si>
+  <si>
+    <t>half uur te laat, goed gewerkt</t>
+  </si>
+  <si>
+    <t>goed bezig, was de enige die feedback op mij gaf nadat ik het vroeg heb de feedback opgenomen</t>
+  </si>
+  <si>
+    <t>Erwin en Paco een half uur te laat</t>
+  </si>
+  <si>
+    <t>Ziekenhuis controlle</t>
+  </si>
+  <si>
+    <t>Greenlight presentation</t>
+  </si>
+  <si>
+    <t>Ziekenhuis</t>
   </si>
 </sst>
 </file>
@@ -449,7 +479,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -527,6 +557,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -799,7 +835,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -1152,6 +1188,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1428,7 +1480,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1438,8 +1490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N75" sqref="N75"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N84" sqref="M82:O87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1447,20 +1499,20 @@
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="10.88671875" style="114" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.6640625" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="29.44140625" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.88671875" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="10.88671875" style="114" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="10.88671875" style="114" customWidth="1"/>
+    <col min="8" max="8" width="29.44140625" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="10.88671875" style="114" customWidth="1"/>
     <col min="10" max="10" width="30.21875" style="114" customWidth="1" outlineLevel="1"/>
     <col min="11" max="11" width="10.88671875" style="114" customWidth="1"/>
     <col min="12" max="12" width="28.33203125" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="13" max="13" width="10.88671875" style="114" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="35.44140625" style="114" customWidth="1" outlineLevel="1"/>
     <col min="15" max="15" width="10.88671875" style="114" customWidth="1"/>
-    <col min="16" max="16" width="40" style="114" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="42.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="40" style="114" customWidth="1" outlineLevel="1"/>
+    <col min="17" max="17" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="27.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="22.109375" style="7" customWidth="1"/>
     <col min="20" max="20" width="25.33203125" style="14" bestFit="1" customWidth="1"/>
@@ -1534,15 +1586,15 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="46">
         <f>B8+B16+B24+B32+B47+B55+B63+B71+B79+B87+B95+B103+B118+B126+B134+B142+B150+B158+B166+B174</f>
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="S2" s="62">
         <f>C8+C16+C24+C32+C47+C55+C63+C71+C79+C87+C95+C103+C118+C126+C134+C142+C150+C158+C166+C174</f>
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="T2" s="68">
         <f>S2/R2</f>
-        <v>0.97540983606557374</v>
+        <v>0.97619047619047616</v>
       </c>
       <c r="U2" s="57" t="str">
         <f>C1</f>
@@ -1602,11 +1654,11 @@
       <c r="R3" s="10"/>
       <c r="S3" s="63">
         <f>E8+E16+E24+E32+E47+E55+E63+E71+E79+E87+E95+E103+E118+E126+E134+E142+E150+E158+E166+E174</f>
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="T3" s="69">
         <f>S3/R2</f>
-        <v>0.84426229508196726</v>
+        <v>0.84920634920634919</v>
       </c>
       <c r="U3" s="58" t="str">
         <f>E1</f>
@@ -1666,11 +1718,11 @@
       <c r="R4" s="10"/>
       <c r="S4" s="64">
         <f>G8+G16+G24+G32+G47+G55+G63+G71+G79+G87+G95+G103+G118+G126+G134+G142+G150+G158+G166+G174</f>
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="T4" s="70">
         <f>S4/R2</f>
-        <v>0.95081967213114749</v>
+        <v>0.95238095238095233</v>
       </c>
       <c r="U4" s="59" t="str">
         <f>G1</f>
@@ -1730,11 +1782,11 @@
       <c r="R5" s="10"/>
       <c r="S5" s="65">
         <f>I8+I16+I24+I32+I47+I55+I63+I71+I79+I87+I95+I103+I118+I126+I134+I142+I150+I158+I166+I174</f>
-        <v>119.5</v>
+        <v>123.5</v>
       </c>
       <c r="T5" s="71">
         <f>S5/R2</f>
-        <v>0.97950819672131151</v>
+        <v>0.98015873015873012</v>
       </c>
       <c r="U5" s="60" t="str">
         <f>I1</f>
@@ -1794,7 +1846,7 @@
       <c r="R6" s="10"/>
       <c r="S6" s="66">
         <f>K8+K16+K24+K32+K47+K55+K63+K71+K79+K87+K95+K103+K118+K126+K134+K142+K150+K158+K166+K174</f>
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="T6" s="72">
         <f>S6/R2</f>
@@ -1850,11 +1902,11 @@
       <c r="R7" s="10"/>
       <c r="S7" s="67">
         <f>M8+M87+M24+M32+M47+M55+M63+M71+M79+M95+M103+M118+M126+M134+M142+M150+M158+M166+M174+M16</f>
-        <v>113.65</v>
+        <v>117.65</v>
       </c>
       <c r="T7" s="73">
         <f>S7/R2</f>
-        <v>0.9315573770491804</v>
+        <v>0.93373015873015874</v>
       </c>
       <c r="U7" s="61" t="str">
         <f>M1</f>
@@ -1908,11 +1960,11 @@
       <c r="R8" s="10"/>
       <c r="S8" s="52">
         <f>O8+O16+O24+O32+O47+O55+O63+O71+O79+O87+O95+O103+O118+O126+O134+O142+O150+O158+O166+O174</f>
-        <v>97.75</v>
+        <v>101.75</v>
       </c>
       <c r="T8" s="53">
         <f>S8/R2</f>
-        <v>0.80122950819672134</v>
+        <v>0.80753968253968256</v>
       </c>
       <c r="U8" s="56" t="str">
         <f>O1</f>
@@ -1962,7 +2014,7 @@
       </c>
       <c r="T10" s="41">
         <f>SUM(T2:T9)</f>
-        <v>6.4827868852459014</v>
+        <v>6.4992063492063492</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4297,7 +4349,7 @@
         <v>3.75</v>
       </c>
       <c r="P70" s="107" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="Q70" s="28" t="s">
         <v>120</v>
@@ -4398,20 +4450,26 @@
       <c r="C74" s="48">
         <v>4</v>
       </c>
-      <c r="D74" s="49"/>
+      <c r="D74" s="49" t="s">
+        <v>87</v>
+      </c>
       <c r="E74" s="49">
         <v>4</v>
       </c>
-      <c r="F74" s="49"/>
+      <c r="F74" s="49" t="s">
+        <v>87</v>
+      </c>
       <c r="G74" s="49">
         <v>4</v>
       </c>
-      <c r="H74" s="49"/>
+      <c r="H74" s="49" t="s">
+        <v>87</v>
+      </c>
       <c r="I74" s="49">
         <v>3.5</v>
       </c>
       <c r="J74" s="49" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="K74" s="49">
         <v>4</v>
@@ -4421,46 +4479,60 @@
         <v>3.5</v>
       </c>
       <c r="N74" s="49" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="O74" s="50">
         <v>4</v>
       </c>
       <c r="P74" s="50"/>
-      <c r="Q74" s="2"/>
+      <c r="Q74" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="R74" s="10"/>
     </row>
     <row r="75" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B75" s="10"/>
+      <c r="B75" s="10">
+        <v>4</v>
+      </c>
       <c r="C75" s="48">
-        <v>0</v>
-      </c>
-      <c r="D75" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="D75" s="49" t="s">
+        <v>124</v>
+      </c>
       <c r="E75" s="49">
-        <v>0</v>
-      </c>
-      <c r="F75" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="F75" s="49" t="s">
+        <v>125</v>
+      </c>
       <c r="G75" s="49">
-        <v>0</v>
-      </c>
-      <c r="H75" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="H75" s="49" t="s">
+        <v>126</v>
+      </c>
       <c r="I75" s="49">
-        <v>0</v>
-      </c>
-      <c r="J75" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="J75" s="49" t="s">
+        <v>87</v>
+      </c>
       <c r="K75" s="49">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L75" s="49"/>
       <c r="M75" s="49">
-        <v>0</v>
-      </c>
-      <c r="N75" s="49"/>
+        <v>4</v>
+      </c>
+      <c r="N75" s="49" t="s">
+        <v>128</v>
+      </c>
       <c r="O75" s="50">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P75" s="50"/>
       <c r="Q75" s="2"/>
@@ -4486,7 +4558,9 @@
       <c r="I76" s="49">
         <v>0</v>
       </c>
-      <c r="J76" s="49"/>
+      <c r="J76" s="49" t="s">
+        <v>130</v>
+      </c>
       <c r="K76" s="49">
         <v>0</v>
       </c>
@@ -4580,47 +4654,47 @@
       </c>
       <c r="B79" s="46">
         <f>SUM(B74:B78)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C79" s="90">
         <f t="shared" ref="C79:K79" si="8">SUM(C74:C78)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D79" s="91"/>
       <c r="E79" s="91">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F79" s="91"/>
       <c r="G79" s="91">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H79" s="91"/>
       <c r="I79" s="91">
         <f t="shared" si="8"/>
-        <v>3.5</v>
+        <v>7.5</v>
       </c>
       <c r="J79" s="91"/>
       <c r="K79" s="91">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L79" s="91"/>
       <c r="M79" s="91">
         <f>SUM(M74:M78)</f>
-        <v>3.5</v>
+        <v>7.5</v>
       </c>
       <c r="N79" s="91"/>
       <c r="O79" s="92">
         <f>SUM(O74:O78)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P79" s="92"/>
       <c r="Q79" s="44"/>
       <c r="R79" s="10"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C80" s="93"/>
       <c r="D80" s="93"/>
       <c r="E80" s="93"/>
@@ -4636,7 +4710,7 @@
       <c r="O80" s="93"/>
       <c r="P80" s="93"/>
     </row>
-    <row r="81" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>21</v>
       </c>
@@ -4658,7 +4732,7 @@
       <c r="Q81" s="1"/>
       <c r="R81" s="10"/>
     </row>
-    <row r="82" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
         <v>0</v>
       </c>
@@ -4694,7 +4768,7 @@
       <c r="Q82" s="2"/>
       <c r="R82" s="10"/>
     </row>
-    <row r="83" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
         <v>1</v>
       </c>
@@ -4722,7 +4796,9 @@
       <c r="M83" s="49">
         <v>0</v>
       </c>
-      <c r="N83" s="49"/>
+      <c r="N83" s="49" t="s">
+        <v>132</v>
+      </c>
       <c r="O83" s="50">
         <v>0</v>
       </c>
@@ -4730,7 +4806,7 @@
       <c r="Q83" s="2"/>
       <c r="R83" s="10"/>
     </row>
-    <row r="84" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="s">
         <v>2</v>
       </c>
@@ -4766,7 +4842,7 @@
       <c r="Q84" s="2"/>
       <c r="R84" s="10"/>
     </row>
-    <row r="85" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
         <v>3</v>
       </c>
@@ -4802,7 +4878,7 @@
       <c r="Q85" s="2"/>
       <c r="R85" s="10"/>
     </row>
-    <row r="86" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="6" t="s">
         <v>4</v>
       </c>
@@ -4838,7 +4914,7 @@
       <c r="Q86" s="3"/>
       <c r="R86" s="10"/>
     </row>
-    <row r="87" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="6" t="s">
         <v>5</v>
       </c>
@@ -4883,7 +4959,7 @@
       <c r="Q87" s="44"/>
       <c r="R87" s="10"/>
     </row>
-    <row r="88" spans="1:18" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C88" s="93"/>
       <c r="D88" s="93"/>
       <c r="E88" s="93"/>
@@ -4899,7 +4975,7 @@
       <c r="O88" s="93"/>
       <c r="P88" s="93"/>
     </row>
-    <row r="89" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>22</v>
       </c>
@@ -4921,7 +4997,7 @@
       <c r="Q89" s="1"/>
       <c r="R89" s="10"/>
     </row>
-    <row r="90" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
         <v>0</v>
       </c>
@@ -4957,7 +5033,7 @@
       <c r="Q90" s="2"/>
       <c r="R90" s="10"/>
     </row>
-    <row r="91" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
         <v>1</v>
       </c>
@@ -4993,7 +5069,7 @@
       <c r="Q91" s="2"/>
       <c r="R91" s="10"/>
     </row>
-    <row r="92" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A92" s="5" t="s">
         <v>2</v>
       </c>
@@ -5029,7 +5105,7 @@
       <c r="Q92" s="2"/>
       <c r="R92" s="10"/>
     </row>
-    <row r="93" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A93" s="5" t="s">
         <v>3</v>
       </c>
@@ -5065,7 +5141,7 @@
       <c r="Q93" s="2"/>
       <c r="R93" s="10"/>
     </row>
-    <row r="94" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="6" t="s">
         <v>4</v>
       </c>
@@ -5101,7 +5177,7 @@
       <c r="Q94" s="3"/>
       <c r="R94" s="10"/>
     </row>
-    <row r="95" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A95" s="6" t="s">
         <v>5</v>
       </c>
@@ -5146,7 +5222,8 @@
       <c r="Q95" s="44"/>
       <c r="R95" s="10"/>
     </row>
-    <row r="96" spans="1:18" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="143"/>
       <c r="C96" s="93"/>
       <c r="D96" s="93"/>
       <c r="E96" s="93"/>
@@ -5162,29 +5239,31 @@
       <c r="O96" s="93"/>
       <c r="P96" s="93"/>
     </row>
-    <row r="97" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="4" t="s">
+    <row r="97" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="142" t="s">
         <v>23</v>
       </c>
-      <c r="B97" s="8"/>
-      <c r="C97" s="87"/>
-      <c r="D97" s="88"/>
-      <c r="E97" s="88"/>
-      <c r="F97" s="88"/>
-      <c r="G97" s="88"/>
-      <c r="H97" s="88"/>
-      <c r="I97" s="88"/>
-      <c r="J97" s="88"/>
-      <c r="K97" s="88"/>
-      <c r="L97" s="88"/>
-      <c r="M97" s="88"/>
-      <c r="N97" s="88"/>
-      <c r="O97" s="89"/>
-      <c r="P97" s="89"/>
-      <c r="Q97" s="1"/>
+      <c r="B97" s="144" t="s">
+        <v>131</v>
+      </c>
+      <c r="C97" s="138"/>
+      <c r="D97" s="139"/>
+      <c r="E97" s="139"/>
+      <c r="F97" s="139"/>
+      <c r="G97" s="139"/>
+      <c r="H97" s="139"/>
+      <c r="I97" s="139"/>
+      <c r="J97" s="139"/>
+      <c r="K97" s="139"/>
+      <c r="L97" s="139"/>
+      <c r="M97" s="139"/>
+      <c r="N97" s="139"/>
+      <c r="O97" s="140"/>
+      <c r="P97" s="140"/>
+      <c r="Q97" s="141"/>
       <c r="R97" s="10"/>
     </row>
-    <row r="98" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="s">
         <v>0</v>
       </c>
@@ -5220,7 +5299,7 @@
       <c r="Q98" s="2"/>
       <c r="R98" s="10"/>
     </row>
-    <row r="99" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
         <v>1</v>
       </c>
@@ -5256,8 +5335,8 @@
       <c r="Q99" s="2"/>
       <c r="R99" s="10"/>
     </row>
-    <row r="100" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="5" t="s">
+    <row r="100" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="145" t="s">
         <v>2</v>
       </c>
       <c r="B100" s="10"/>
@@ -5292,7 +5371,7 @@
       <c r="Q100" s="2"/>
       <c r="R100" s="10"/>
     </row>
-    <row r="101" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="s">
         <v>3</v>
       </c>
@@ -5328,7 +5407,7 @@
       <c r="Q101" s="2"/>
       <c r="R101" s="10"/>
     </row>
-    <row r="102" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="6" t="s">
         <v>4</v>
       </c>
@@ -5364,7 +5443,7 @@
       <c r="Q102" s="3"/>
       <c r="R102" s="10"/>
     </row>
-    <row r="103" spans="1:18" ht="15" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:18" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103" s="6" t="s">
         <v>5</v>
       </c>
@@ -5409,7 +5488,7 @@
       <c r="Q103" s="39"/>
       <c r="R103" s="10"/>
     </row>
-    <row r="104" spans="1:18" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C104" s="93"/>
       <c r="D104" s="93"/>
       <c r="E104" s="93"/>

</xml_diff>

<commit_message>
Bug log & Presentation
</commit_message>
<xml_diff>
--- a/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
+++ b/Algemeen/Uren Registratie Game-Lab-2.1.xlsx
@@ -1583,7 +1583,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1593,8 +1593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U182"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C184" sqref="C184"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q188" sqref="Q188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1667,7 +1667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>Roos</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>Harold</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>Patrick</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>Erwin</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>Sven</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>Paco</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>Danial</v>
       </c>
     </row>
-    <row r="9" spans="1:21" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C9" s="93"/>
       <c r="D9" s="93"/>
       <c r="E9" s="93"/>
@@ -8739,37 +8739,37 @@
         <v>4</v>
       </c>
       <c r="C182" s="90">
-        <f t="shared" ref="C182:O182" si="20">SUM(C177:C181)</f>
+        <f t="shared" ref="C182" si="20">SUM(C177:C181)</f>
         <v>4</v>
       </c>
       <c r="D182" s="91"/>
       <c r="E182" s="91">
-        <f t="shared" ref="E182:Q182" si="21">SUM(E177:E181)</f>
+        <f t="shared" ref="E182" si="21">SUM(E177:E181)</f>
         <v>4</v>
       </c>
       <c r="F182" s="91"/>
       <c r="G182" s="91">
-        <f t="shared" ref="G182:Q182" si="22">SUM(G177:G181)</f>
+        <f t="shared" ref="G182" si="22">SUM(G177:G181)</f>
         <v>4</v>
       </c>
       <c r="H182" s="91"/>
       <c r="I182" s="91">
-        <f t="shared" ref="I182:Q182" si="23">SUM(I177:I181)</f>
+        <f t="shared" ref="I182" si="23">SUM(I177:I181)</f>
         <v>4</v>
       </c>
       <c r="J182" s="91"/>
       <c r="K182" s="91">
-        <f t="shared" ref="K182:Q182" si="24">SUM(K177:K181)</f>
+        <f t="shared" ref="K182" si="24">SUM(K177:K181)</f>
         <v>4</v>
       </c>
       <c r="L182" s="91"/>
       <c r="M182" s="91">
-        <f t="shared" ref="M182:Q182" si="25">SUM(M177:M181)</f>
+        <f t="shared" ref="M182" si="25">SUM(M177:M181)</f>
         <v>4</v>
       </c>
       <c r="N182" s="91"/>
       <c r="O182" s="91">
-        <f t="shared" ref="O182:Q182" si="26">SUM(O177:O181)</f>
+        <f t="shared" ref="O182" si="26">SUM(O177:O181)</f>
         <v>4</v>
       </c>
       <c r="P182" s="91"/>

</xml_diff>